<commit_message>
Various updates in cluding fixing body, spell damage and duplicate craftable items.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Weapons/spell_damage.xlsx
+++ b/resources/data-imports/Weapons/spell_damage.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="187">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -883,8 +883,8 @@
   </sheetPr>
   <dimension ref="A1:BN60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2:K60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6694,17 +6694,86 @@
       <c r="K60" s="3" t="n">
         <v>35999071473</v>
       </c>
+      <c r="N60" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="V60" s="1" t="n">
         <v>0.272333511685371</v>
       </c>
+      <c r="W60" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="X60" s="1" t="n">
         <v>0.272333511685371</v>
       </c>
+      <c r="Z60" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="AB60" s="1" t="n">
         <v>389</v>
       </c>
       <c r="AC60" s="1" t="n">
         <v>401</v>
+      </c>
+      <c r="AD60" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM60" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW60" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AX60" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AY60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ60" s="1" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed type on the spell damage
</commit_message>
<xml_diff>
--- a/resources/data-imports/Weapons/spell_damage.xlsx
+++ b/resources/data-imports/Weapons/spell_damage.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="186">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -575,9 +575,6 @@
   </si>
   <si>
     <t xml:space="preserve">Demonic Invocation of Deaths Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spell-damage</t>
   </si>
   <si>
     <t xml:space="preserve">A horrific demonic invocation of death in his name. Let the king of death rip through your enemies souls</t>
@@ -884,7 +881,7 @@
   <dimension ref="A1:BN60"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
+      <selection pane="topLeft" activeCell="D60" activeCellId="0" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6683,10 +6680,10 @@
         <v>184</v>
       </c>
       <c r="D60" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="H60" s="1" t="n">
         <v>1000</v>

</xml_diff>